<commit_message>
update of input sheets for tests
</commit_message>
<xml_diff>
--- a/tests/testdata/test_geometry_material_input.xlsx
+++ b/tests/testdata/test_geometry_material_input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="Input_variables" sheetId="1" r:id="rId1"/>
@@ -1767,17 +1767,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="A11:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="46" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" customWidth="1"/>
-    <col min="4" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.453125" customWidth="1"/>
+    <col min="4" max="6" width="19.453125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="17.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -2022,486 +2022,486 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="40"/>
-      <c r="B11" t="s">
-        <v>93</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D11" s="2">
-        <v>100000</v>
-      </c>
-      <c r="E11" s="2">
-        <v>100000</v>
-      </c>
-      <c r="F11" s="2">
-        <v>100000</v>
-      </c>
-      <c r="G11" s="2">
-        <v>100000</v>
-      </c>
-      <c r="H11" s="2">
-        <v>100000</v>
+    <row r="11" spans="1:8" ht="15" customHeight="1">
+      <c r="A11" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11">
+        <v>24.9397924881983</v>
+      </c>
+      <c r="E11">
+        <v>29.846033506748501</v>
+      </c>
+      <c r="F11">
+        <v>21.549071913738601</v>
+      </c>
+      <c r="G11">
+        <v>30.724628045371599</v>
+      </c>
+      <c r="H11">
+        <v>24.603567265875999</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="40"/>
-      <c r="B12" t="s">
-        <v>94</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="D12" s="2">
-        <v>500000</v>
-      </c>
-      <c r="E12" s="2">
-        <v>500000</v>
-      </c>
-      <c r="F12" s="2">
-        <v>800000</v>
-      </c>
-      <c r="G12" s="2">
-        <v>100000</v>
-      </c>
-      <c r="H12" s="2">
-        <v>200000</v>
+      <c r="A12" s="41"/>
+      <c r="B12" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12">
+        <v>0.397534327540081</v>
+      </c>
+      <c r="E12">
+        <v>0.38745672969163403</v>
+      </c>
+      <c r="F12">
+        <v>0.27778552720397198</v>
+      </c>
+      <c r="G12">
+        <v>0.38853068564494597</v>
+      </c>
+      <c r="H12">
+        <v>0.39281645770158102</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="40"/>
+      <c r="A13" s="41"/>
       <c r="B13" t="s">
-        <v>95</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>84</v>
+        <v>42</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>310.53423258511901</v>
       </c>
       <c r="E13">
-        <v>2</v>
+        <v>311.82631932244198</v>
       </c>
       <c r="F13">
-        <v>4</v>
+        <v>262.54231664112598</v>
       </c>
       <c r="G13">
-        <v>1</v>
+        <v>334.01554867815503</v>
       </c>
       <c r="H13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1">
-      <c r="A14" s="41" t="s">
-        <v>140</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>37</v>
+        <v>217.83710715883799</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="41"/>
+      <c r="B14" t="s">
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D14">
-        <v>24.9397924881983</v>
+        <v>0.43852951083798603</v>
       </c>
       <c r="E14">
-        <v>29.846033506748501</v>
+        <v>0.27896020164795099</v>
       </c>
       <c r="F14">
-        <v>21.549071913738601</v>
+        <v>0.41639127372561502</v>
       </c>
       <c r="G14">
-        <v>30.724628045371599</v>
+        <v>0.36908011038102101</v>
       </c>
       <c r="H14">
-        <v>24.603567265875999</v>
+        <v>0.33759378483001701</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="41"/>
-      <c r="B15" s="11" t="s">
-        <v>39</v>
+      <c r="B15" t="s">
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D15">
-        <v>0.397534327540081</v>
+        <v>9592.8821295104699</v>
       </c>
       <c r="E15">
-        <v>0.38745672969163403</v>
+        <v>13728.6250951821</v>
       </c>
       <c r="F15">
-        <v>0.27778552720397198</v>
+        <v>9530.9428397424908</v>
       </c>
       <c r="G15">
-        <v>0.38853068564494597</v>
+        <v>11844.471056845599</v>
       </c>
       <c r="H15">
-        <v>0.39281645770158102</v>
+        <v>7039.1850549506698</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="41"/>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D16">
-        <v>310.53423258511901</v>
+        <v>6.9859353305379797</v>
       </c>
       <c r="E16">
-        <v>311.82631932244198</v>
+        <v>4.8667038063889603</v>
       </c>
       <c r="F16">
-        <v>262.54231664112598</v>
+        <v>5.9682746322479998</v>
       </c>
       <c r="G16">
-        <v>334.01554867815503</v>
+        <v>7.6920989582716999</v>
       </c>
       <c r="H16">
-        <v>217.83710715883799</v>
+        <v>7.9973902757422897</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="41"/>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D17">
-        <v>0.43852951083798603</v>
+        <v>0.36032232455732299</v>
       </c>
       <c r="E17">
-        <v>0.27896020164795099</v>
+        <v>0.43263553136410199</v>
       </c>
       <c r="F17">
-        <v>0.41639127372561502</v>
+        <v>0.311870213321776</v>
       </c>
       <c r="G17">
-        <v>0.36908011038102101</v>
+        <v>0.34484796209278801</v>
       </c>
       <c r="H17">
-        <v>0.33759378483001701</v>
+        <v>0.43685550941856799</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="41"/>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="D18">
-        <v>9592.8821295104699</v>
+        <v>235.360704664796</v>
       </c>
       <c r="E18">
-        <v>13728.6250951821</v>
+        <v>208.806759033595</v>
       </c>
       <c r="F18">
-        <v>9530.9428397424908</v>
+        <v>226.06765407211699</v>
       </c>
       <c r="G18">
-        <v>11844.471056845599</v>
+        <v>392.86734368371702</v>
       </c>
       <c r="H18">
-        <v>7039.1850549506698</v>
+        <v>391.55736926069602</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="41"/>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D19">
-        <v>6.9859353305379797</v>
+        <v>3620.8448324163101</v>
       </c>
       <c r="E19">
-        <v>4.8667038063889603</v>
+        <v>2311.15858694705</v>
       </c>
       <c r="F19">
-        <v>5.9682746322479998</v>
+        <v>2343.2994179618399</v>
       </c>
       <c r="G19">
-        <v>7.6920989582716999</v>
+        <v>4284.9699230713404</v>
       </c>
       <c r="H19">
-        <v>7.9973902757422897</v>
+        <v>3659.2272904198899</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="41"/>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D20">
-        <v>0.36032232455732299</v>
+        <v>1.13373577673032</v>
       </c>
       <c r="E20">
-        <v>0.43263553136410199</v>
+        <v>2.4258179969420199</v>
       </c>
       <c r="F20">
-        <v>0.311870213321776</v>
+        <v>2.3873285971102698</v>
       </c>
       <c r="G20">
-        <v>0.34484796209278801</v>
+        <v>1.4564750409017799</v>
       </c>
       <c r="H20">
-        <v>0.43685550941856799</v>
+        <v>0.99721191005946297</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="41"/>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C21" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D21">
-        <v>235.360704664796</v>
+        <v>0.67575877439752896</v>
       </c>
       <c r="E21">
-        <v>208.806759033595</v>
+        <v>0.51712000434017502</v>
       </c>
       <c r="F21">
-        <v>226.06765407211699</v>
+        <v>0.801477721483979</v>
       </c>
       <c r="G21">
-        <v>392.86734368371702</v>
+        <v>9.8010774605840997E-2</v>
       </c>
       <c r="H21">
-        <v>391.55736926069602</v>
+        <v>0.74159415955053198</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="41"/>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C22" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D22">
-        <v>3620.8448324163101</v>
+        <v>3.8387980542432998</v>
       </c>
       <c r="E22">
-        <v>2311.15858694705</v>
+        <v>1.8776339003870799</v>
       </c>
       <c r="F22">
-        <v>2343.2994179618399</v>
+        <v>3.3657208787845398</v>
       </c>
       <c r="G22">
-        <v>4284.9699230713404</v>
+        <v>2.4178541756165899</v>
       </c>
       <c r="H22">
-        <v>3659.2272904198899</v>
+        <v>1.56466211459187</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="41"/>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C23" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D23">
-        <v>1.13373577673032</v>
+        <v>0.82317441160238602</v>
       </c>
       <c r="E23">
-        <v>2.4258179969420199</v>
+        <v>0.63680145228157503</v>
       </c>
       <c r="F23">
-        <v>2.3873285971102698</v>
+        <v>0.85382760203728802</v>
       </c>
       <c r="G23">
-        <v>1.4564750409017799</v>
+        <v>0.594424181188418</v>
       </c>
       <c r="H23">
-        <v>0.99721191005946297</v>
+        <v>0.58201942471427504</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="41"/>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C24" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D24">
-        <v>0.67575877439752896</v>
+        <v>2351.0358557609202</v>
       </c>
       <c r="E24">
-        <v>0.51712000434017502</v>
+        <v>4305.6905785423696</v>
       </c>
       <c r="F24">
-        <v>0.801477721483979</v>
+        <v>5592.7916508867802</v>
       </c>
       <c r="G24">
-        <v>9.8010774605840997E-2</v>
+        <v>1093.0004954073299</v>
       </c>
       <c r="H24">
-        <v>0.74159415955053198</v>
+        <v>5316.4232733114604</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="41"/>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C25" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D25">
-        <v>3.8387980542432998</v>
+        <v>479.56427978543297</v>
       </c>
       <c r="E25">
-        <v>1.8776339003870799</v>
+        <v>342.07526272382</v>
       </c>
       <c r="F25">
-        <v>3.3657208787845398</v>
+        <v>629.09549703360005</v>
       </c>
       <c r="G25">
-        <v>2.4178541756165899</v>
+        <v>1336.8970567521501</v>
       </c>
       <c r="H25">
-        <v>1.56466211459187</v>
+        <v>1431.3338377950799</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="41"/>
       <c r="B26" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C26" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D26">
-        <v>0.82317441160238602</v>
+        <v>1.5209241133552001</v>
       </c>
       <c r="E26">
-        <v>0.63680145228157503</v>
+        <v>1.4611356146706</v>
       </c>
       <c r="F26">
-        <v>0.85382760203728802</v>
+        <v>1.17459338972312</v>
       </c>
       <c r="G26">
-        <v>0.594424181188418</v>
+        <v>1.17980028181748</v>
       </c>
       <c r="H26">
-        <v>0.58201942471427504</v>
+        <v>0.97421919684422997</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="41"/>
       <c r="B27" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C27" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D27">
-        <v>2351.0358557609202</v>
+        <v>148.023377589456</v>
       </c>
       <c r="E27">
-        <v>4305.6905785423696</v>
+        <v>196.39317107510001</v>
       </c>
       <c r="F27">
-        <v>5592.7916508867802</v>
+        <v>170.37252984731199</v>
       </c>
       <c r="G27">
-        <v>1093.0004954073299</v>
+        <v>285.26395874702098</v>
       </c>
       <c r="H27">
-        <v>5316.4232733114604</v>
+        <v>203.71546054260199</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="41"/>
       <c r="B28" t="s">
-        <v>65</v>
-      </c>
-      <c r="C28" t="s">
-        <v>66</v>
-      </c>
-      <c r="D28">
-        <v>479.56427978543297</v>
-      </c>
-      <c r="E28">
-        <v>342.07526272382</v>
-      </c>
-      <c r="F28">
-        <v>629.09549703360005</v>
-      </c>
-      <c r="G28">
-        <v>1336.8970567521501</v>
-      </c>
-      <c r="H28">
-        <v>1431.3338377950799</v>
+        <v>93</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D28" s="2">
+        <v>100000</v>
+      </c>
+      <c r="E28" s="2">
+        <v>100000</v>
+      </c>
+      <c r="F28" s="2">
+        <v>100000</v>
+      </c>
+      <c r="G28" s="2">
+        <v>100000</v>
+      </c>
+      <c r="H28" s="2">
+        <v>100000</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="41"/>
       <c r="B29" t="s">
-        <v>67</v>
-      </c>
-      <c r="C29" t="s">
-        <v>68</v>
-      </c>
-      <c r="D29">
-        <v>1.5209241133552001</v>
-      </c>
-      <c r="E29">
-        <v>1.4611356146706</v>
-      </c>
-      <c r="F29">
-        <v>1.17459338972312</v>
-      </c>
-      <c r="G29">
-        <v>1.17980028181748</v>
-      </c>
-      <c r="H29">
-        <v>0.97421919684422997</v>
+        <v>94</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="D29" s="2">
+        <v>500000</v>
+      </c>
+      <c r="E29" s="2">
+        <v>500000</v>
+      </c>
+      <c r="F29" s="2">
+        <v>800000</v>
+      </c>
+      <c r="G29" s="2">
+        <v>100000</v>
+      </c>
+      <c r="H29" s="2">
+        <v>200000</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="41"/>
       <c r="B30" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="C30" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="D30">
-        <v>148.023377589456</v>
+        <v>1</v>
       </c>
       <c r="E30">
-        <v>196.39317107510001</v>
+        <v>2</v>
       </c>
       <c r="F30">
-        <v>170.37252984731199</v>
+        <v>4</v>
       </c>
       <c r="G30">
-        <v>285.26395874702098</v>
+        <v>1</v>
       </c>
       <c r="H30">
-        <v>203.71546054260199</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -2744,7 +2744,7 @@
         <v>0.94103602888102855</v>
       </c>
       <c r="G40">
-        <f t="shared" ref="G40" si="0">(0.005/G3)^(1/3)</f>
+        <f>(0.005/G3)^(1/3)</f>
         <v>0.94103602888102855</v>
       </c>
       <c r="H40">
@@ -3006,29 +3006,29 @@
         <v>192093.02325581395</v>
       </c>
       <c r="E51">
-        <f t="shared" ref="E51:H51" si="1">(2*E43*E44)/(E43+E44)</f>
+        <f t="shared" ref="E51:H51" si="0">(2*E43*E44)/(E43+E44)</f>
         <v>210000</v>
       </c>
       <c r="F51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>210000</v>
       </c>
       <c r="G51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>210000</v>
       </c>
       <c r="H51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>210000</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A1:A13"/>
-    <mergeCell ref="A14:A30"/>
+    <mergeCell ref="A1:A10"/>
     <mergeCell ref="A31:A33"/>
     <mergeCell ref="A34:A40"/>
     <mergeCell ref="A41:A51"/>
+    <mergeCell ref="A11:A30"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="If the desired material does not figrue on the list, please add it as well as its following parameters to the list in the worksheet &quot;rail and wheel materials&quot;" sqref="D8:H8"/>
@@ -3046,15 +3046,15 @@
       <selection activeCell="I9" sqref="A1:I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.453125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="7" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.7265625" customWidth="1"/>
+    <col min="5" max="6" width="11.453125" customWidth="1"/>
+    <col min="7" max="7" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.25" customHeight="1">
@@ -3086,7 +3086,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="120">
+    <row r="2" spans="1:9" ht="98">
       <c r="A2" s="25" t="s">
         <v>123</v>
       </c>
@@ -3333,19 +3333,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -3377,7 +3377,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="75">
+    <row r="2" spans="1:9" ht="70">
       <c r="A2" s="25" t="s">
         <v>123</v>
       </c>
@@ -3684,7 +3684,7 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="35" t="s">
@@ -3804,7 +3804,7 @@
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="35" t="s">

</xml_diff>